<commit_message>
chutian - temp for 20221130
</commit_message>
<xml_diff>
--- a/miaoTemp/楚天/汉阳用户.xlsx
+++ b/miaoTemp/楚天/汉阳用户.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>姓名</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>预约时间</t>
+  </si>
+  <si>
+    <t>测试</t>
   </si>
   <si>
     <t xml:space="preserve">李梦希 </t>
@@ -1109,7 +1112,7 @@
   <dimension ref="C7:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1165,9 +1168,13 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="3:8">
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="9">
+        <v>17014049717</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1198,10 +1205,10 @@
     </row>
     <row r="15" spans="3:8">
       <c r="C15" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="9">
         <v>17025472447</v>
@@ -1216,10 +1223,10 @@
     </row>
     <row r="16" spans="3:8">
       <c r="C16" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="9">
         <v>17152022762</v>
@@ -1234,10 +1241,10 @@
     </row>
     <row r="17" spans="3:8">
       <c r="C17" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" s="9">
         <v>17198008619</v>
@@ -1252,10 +1259,10 @@
     </row>
     <row r="18" spans="3:8">
       <c r="C18" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="9">
         <v>17054654268</v>
@@ -1270,10 +1277,10 @@
     </row>
     <row r="19" spans="3:8">
       <c r="C19" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="9">
         <v>17147715197</v>
@@ -1288,13 +1295,13 @@
     </row>
     <row r="20" spans="3:8">
       <c r="C20" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="9">
-        <v>17014049717</v>
+        <v>17050685132</v>
       </c>
       <c r="F20" s="10">
         <v>18872055089</v>
@@ -1306,10 +1313,10 @@
     </row>
     <row r="21" spans="3:8">
       <c r="C21" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="6">
         <v>17050685132</v>
@@ -1322,10 +1329,10 @@
     </row>
     <row r="22" spans="3:8">
       <c r="C22" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7">
@@ -1336,10 +1343,10 @@
     </row>
     <row r="23" spans="3:8">
       <c r="C23" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
@@ -1350,10 +1357,10 @@
     </row>
     <row r="24" spans="3:8">
       <c r="C24" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7">
@@ -1364,10 +1371,10 @@
     </row>
     <row r="25" spans="3:8">
       <c r="C25" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="7">
@@ -1378,10 +1385,10 @@
     </row>
     <row r="26" spans="3:8">
       <c r="C26" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="7">
@@ -1392,10 +1399,10 @@
     </row>
     <row r="27" spans="3:8">
       <c r="C27" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="15">
@@ -1406,10 +1413,10 @@
     </row>
     <row r="28" spans="3:8">
       <c r="C28" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="15">

</xml_diff>

<commit_message>
jkzl - auth user idcard
</commit_message>
<xml_diff>
--- a/miaoTemp/楚天/汉阳用户.xlsx
+++ b/miaoTemp/楚天/汉阳用户.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>姓名</t>
   </si>
@@ -31,6 +31,21 @@
     <t>预约时间</t>
   </si>
   <si>
+    <t>张远媛</t>
+  </si>
+  <si>
+    <t>612426199806235426</t>
+  </si>
+  <si>
+    <t>李佳</t>
+  </si>
+  <si>
+    <t>411524199506020022</t>
+  </si>
+  <si>
+    <t>用户说打不了阔龄</t>
+  </si>
+  <si>
     <t>测试</t>
   </si>
   <si>
@@ -56,18 +71,6 @@
   </si>
   <si>
     <t>421023199507142927</t>
-  </si>
-  <si>
-    <t>李佳</t>
-  </si>
-  <si>
-    <t>411524199506020022</t>
-  </si>
-  <si>
-    <t>张远媛</t>
-  </si>
-  <si>
-    <t>612426199806235426</t>
   </si>
   <si>
     <t>晏林</t>
@@ -281,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.35"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,10 +623,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -626,16 +635,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -647,10 +656,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -671,28 +680,28 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -701,19 +710,16 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -725,38 +731,41 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -773,22 +782,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1109,10 +1127,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C7:H42"/>
+  <dimension ref="C7:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1152,24 +1170,46 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="3:8">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9">
+        <v>17050685132</v>
+      </c>
+      <c r="F9" s="10">
+        <v>18872055089</v>
+      </c>
+      <c r="G9" s="11">
+        <v>44895</v>
+      </c>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="3:8">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="C10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12">
+        <v>17147715197</v>
+      </c>
+      <c r="F10" s="13">
+        <v>13545147593</v>
+      </c>
+      <c r="G10" s="14">
+        <v>44895</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="3:8">
       <c r="C11" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="9">
@@ -1204,225 +1244,205 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="3:8">
-      <c r="C15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="C15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="16">
         <v>17025472447</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="17">
         <v>13212734213</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="18">
         <v>44895</v>
       </c>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="3:8">
-      <c r="C16" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="10">
+      <c r="C16" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="16">
         <v>17152022762</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="17">
         <v>13129949932</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="18">
         <v>44895</v>
       </c>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="3:8">
-      <c r="C17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="C17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="16">
         <v>17198008619</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="17">
         <v>15071061492</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="18">
         <v>44895</v>
       </c>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="10">
+      <c r="C18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="16">
         <v>17054654268</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="17">
         <v>17875713686</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="18">
         <v>44895</v>
       </c>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="10">
-        <v>17147715197</v>
-      </c>
-      <c r="F19" s="11">
-        <v>13545147593</v>
-      </c>
-      <c r="G19" s="12">
-        <v>44895</v>
-      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="6">
+        <v>17050685132</v>
+      </c>
+      <c r="F19" s="7">
+        <v>15730080765</v>
+      </c>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="3:8">
-      <c r="C20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="9">
-        <v>17050685132</v>
-      </c>
-      <c r="F20" s="14">
-        <v>18872055089</v>
-      </c>
-      <c r="G20" s="15">
-        <v>44895</v>
-      </c>
+      <c r="C20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7">
+        <v>15871380235</v>
+      </c>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="3:8">
       <c r="C21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="6">
-        <v>17050685132</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="7">
-        <v>15730080765</v>
-      </c>
-      <c r="G21" s="16"/>
+        <v>18153623551</v>
+      </c>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="3:8">
       <c r="C22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7">
-        <v>15871380235</v>
-      </c>
-      <c r="G22" s="16"/>
+        <v>17865815159</v>
+      </c>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="3:8">
       <c r="C23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
-        <v>18153623551</v>
-      </c>
-      <c r="G23" s="16"/>
+        <v>18704601232</v>
+      </c>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="3:8">
       <c r="C24" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7">
-        <v>17865815159</v>
-      </c>
-      <c r="G24" s="16"/>
+        <v>15171980859</v>
+      </c>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="3:8">
       <c r="C25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="7">
-        <v>18704601232</v>
-      </c>
-      <c r="G25" s="16"/>
+        <v>17865815139</v>
+      </c>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="3:8">
       <c r="C26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="7">
-        <v>15171980859</v>
-      </c>
-      <c r="G26" s="16"/>
+        <v>15982066827</v>
+      </c>
+      <c r="G26" s="20"/>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="3:8">
-      <c r="C27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="7">
-        <v>17865815139</v>
-      </c>
-      <c r="G27" s="16"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="3:8">
-      <c r="C28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="7">
-        <v>15982066827</v>
-      </c>
-      <c r="G28" s="16"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="3:8">
@@ -1521,22 +1541,6 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="3:8">
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="3:8">
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
jkzl - searcher filter
</commit_message>
<xml_diff>
--- a/miaoTemp/楚天/汉阳用户.xlsx
+++ b/miaoTemp/楚天/汉阳用户.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="21000" windowHeight="11070"/>
   </bookViews>
   <sheets>
     <sheet name="汉阳" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>姓名</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>370285199612013224</t>
+  </si>
+  <si>
+    <t>密码Se22223333</t>
   </si>
   <si>
     <t>冯书语</t>
@@ -1224,7 +1227,7 @@
   <dimension ref="C7:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1586,13 +1589,13 @@
         <v>43</v>
       </c>
       <c r="E29" s="31">
-        <v>17054654268</v>
-      </c>
-      <c r="F29" s="33">
         <v>15207127787</v>
       </c>
+      <c r="F29" s="33"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="30" spans="3:8">
       <c r="C30" s="10"/>
@@ -1711,10 +1714,10 @@
     </row>
     <row r="11" spans="5:9">
       <c r="E11" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G11" s="10">
         <v>17190092942</v>
@@ -1728,10 +1731,10 @@
     </row>
     <row r="12" spans="5:9">
       <c r="E12" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="10">
         <v>17136341196</v>
@@ -1745,10 +1748,10 @@
     </row>
     <row r="13" spans="5:9">
       <c r="E13" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G13" s="10">
         <v>17040214075</v>
@@ -1762,10 +1765,10 @@
     </row>
     <row r="14" spans="5:9">
       <c r="E14" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G14" s="10">
         <v>17050683431</v>
@@ -1779,10 +1782,10 @@
     </row>
     <row r="15" spans="5:9">
       <c r="E15" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G15" s="10">
         <v>15607045070</v>

</xml_diff>